<commit_message>
Add discussion of DOAGC example.
</commit_message>
<xml_diff>
--- a/examples/counters/DOAGC.xlsx
+++ b/examples/counters/DOAGC.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Counters" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="44">
   <si>
     <t xml:space="preserve">Nationality</t>
   </si>
@@ -153,27 +152,6 @@
   </si>
   <si>
     <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Army</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grouping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAME TURN</t>
   </si>
 </sst>
 </file>
@@ -386,17 +364,18 @@
   </sheetPr>
   <dimension ref="A1:AMJ201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B159" activeCellId="0" sqref="B159"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="LX1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="LX1" activeCellId="0" sqref="LX1"/>
+      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="647" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,6 +400,384 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="XR1" s="0"/>
+      <c r="XS1" s="0"/>
+      <c r="XT1" s="0"/>
+      <c r="XU1" s="0"/>
+      <c r="XV1" s="0"/>
+      <c r="XW1" s="0"/>
+      <c r="XX1" s="0"/>
+      <c r="XY1" s="0"/>
+      <c r="XZ1" s="0"/>
+      <c r="YA1" s="0"/>
+      <c r="YB1" s="0"/>
+      <c r="YC1" s="0"/>
+      <c r="YD1" s="0"/>
+      <c r="YE1" s="0"/>
+      <c r="YF1" s="0"/>
+      <c r="YG1" s="0"/>
+      <c r="YH1" s="0"/>
+      <c r="YI1" s="0"/>
+      <c r="YJ1" s="0"/>
+      <c r="YK1" s="0"/>
+      <c r="YL1" s="0"/>
+      <c r="YM1" s="0"/>
+      <c r="YN1" s="0"/>
+      <c r="YO1" s="0"/>
+      <c r="YP1" s="0"/>
+      <c r="YQ1" s="0"/>
+      <c r="YR1" s="0"/>
+      <c r="YS1" s="0"/>
+      <c r="YT1" s="0"/>
+      <c r="YU1" s="0"/>
+      <c r="YV1" s="0"/>
+      <c r="YW1" s="0"/>
+      <c r="YX1" s="0"/>
+      <c r="YY1" s="0"/>
+      <c r="YZ1" s="0"/>
+      <c r="ZA1" s="0"/>
+      <c r="ZB1" s="0"/>
+      <c r="ZC1" s="0"/>
+      <c r="ZD1" s="0"/>
+      <c r="ZE1" s="0"/>
+      <c r="ZF1" s="0"/>
+      <c r="ZG1" s="0"/>
+      <c r="ZH1" s="0"/>
+      <c r="ZI1" s="0"/>
+      <c r="ZJ1" s="0"/>
+      <c r="ZK1" s="0"/>
+      <c r="ZL1" s="0"/>
+      <c r="ZM1" s="0"/>
+      <c r="ZN1" s="0"/>
+      <c r="ZO1" s="0"/>
+      <c r="ZP1" s="0"/>
+      <c r="ZQ1" s="0"/>
+      <c r="ZR1" s="0"/>
+      <c r="ZS1" s="0"/>
+      <c r="ZT1" s="0"/>
+      <c r="ZU1" s="0"/>
+      <c r="ZV1" s="0"/>
+      <c r="ZW1" s="0"/>
+      <c r="ZX1" s="0"/>
+      <c r="ZY1" s="0"/>
+      <c r="ZZ1" s="0"/>
+      <c r="AAA1" s="0"/>
+      <c r="AAB1" s="0"/>
+      <c r="AAC1" s="0"/>
+      <c r="AAD1" s="0"/>
+      <c r="AAE1" s="0"/>
+      <c r="AAF1" s="0"/>
+      <c r="AAG1" s="0"/>
+      <c r="AAH1" s="0"/>
+      <c r="AAI1" s="0"/>
+      <c r="AAJ1" s="0"/>
+      <c r="AAK1" s="0"/>
+      <c r="AAL1" s="0"/>
+      <c r="AAM1" s="0"/>
+      <c r="AAN1" s="0"/>
+      <c r="AAO1" s="0"/>
+      <c r="AAP1" s="0"/>
+      <c r="AAQ1" s="0"/>
+      <c r="AAR1" s="0"/>
+      <c r="AAS1" s="0"/>
+      <c r="AAT1" s="0"/>
+      <c r="AAU1" s="0"/>
+      <c r="AAV1" s="0"/>
+      <c r="AAW1" s="0"/>
+      <c r="AAX1" s="0"/>
+      <c r="AAY1" s="0"/>
+      <c r="AAZ1" s="0"/>
+      <c r="ABA1" s="0"/>
+      <c r="ABB1" s="0"/>
+      <c r="ABC1" s="0"/>
+      <c r="ABD1" s="0"/>
+      <c r="ABE1" s="0"/>
+      <c r="ABF1" s="0"/>
+      <c r="ABG1" s="0"/>
+      <c r="ABH1" s="0"/>
+      <c r="ABI1" s="0"/>
+      <c r="ABJ1" s="0"/>
+      <c r="ABK1" s="0"/>
+      <c r="ABL1" s="0"/>
+      <c r="ABM1" s="0"/>
+      <c r="ABN1" s="0"/>
+      <c r="ABO1" s="0"/>
+      <c r="ABP1" s="0"/>
+      <c r="ABQ1" s="0"/>
+      <c r="ABR1" s="0"/>
+      <c r="ABS1" s="0"/>
+      <c r="ABT1" s="0"/>
+      <c r="ABU1" s="0"/>
+      <c r="ABV1" s="0"/>
+      <c r="ABW1" s="0"/>
+      <c r="ABX1" s="0"/>
+      <c r="ABY1" s="0"/>
+      <c r="ABZ1" s="0"/>
+      <c r="ACA1" s="0"/>
+      <c r="ACB1" s="0"/>
+      <c r="ACC1" s="0"/>
+      <c r="ACD1" s="0"/>
+      <c r="ACE1" s="0"/>
+      <c r="ACF1" s="0"/>
+      <c r="ACG1" s="0"/>
+      <c r="ACH1" s="0"/>
+      <c r="ACI1" s="0"/>
+      <c r="ACJ1" s="0"/>
+      <c r="ACK1" s="0"/>
+      <c r="ACL1" s="0"/>
+      <c r="ACM1" s="0"/>
+      <c r="ACN1" s="0"/>
+      <c r="ACO1" s="0"/>
+      <c r="ACP1" s="0"/>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -4351,1957 +4708,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G101"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G101" activeCellId="0" sqref="G101"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E22" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>53</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>54</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D27" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D29" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D30" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>58</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D31" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" s="5" t="n">
-        <v>59</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E37" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E38" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E39" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D42" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E42" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D43" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E43" s="5" t="n">
-        <v>71</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D44" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E44" s="5" t="n">
-        <v>72</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D45" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E45" s="5" t="n">
-        <v>73</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D46" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E46" s="5" t="n">
-        <v>74</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D47" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E47" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D48" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E48" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D49" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E49" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D50" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E50" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D51" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E51" s="5" t="n">
-        <v>82</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E52" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E53" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D54" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E54" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D55" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E55" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D56" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E56" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D57" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E57" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E58" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D62" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C63" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D63" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D64" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D65" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D66" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D67" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D69" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D70" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D71" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E71" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D73" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D74" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D75" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D76" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E76" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D77" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D78" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D79" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E79" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="1"/>
-      <c r="G80" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D82" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E82" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B83" s="4"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D85" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E85" s="5" t="n">
-        <v>131</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D86" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E86" s="5" t="n">
-        <v>367</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D87" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E87" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C88" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D88" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E88" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B89" s="4"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D91" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C92" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D92" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C94" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D94" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E94" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D95" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C96" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D96" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E96" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C97" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D97" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E97" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C98" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D98" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E98" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G99" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D100" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D101" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
More changes & updates (#14)
* Code refactoring

* Add Cube

* Add discussion of DOAGC example.

* Shift data loading to loadr module

* Add Extract command

* Add TM:Ares player board

* Renamed hatch_width to hatch_stroke_width
</commit_message>
<xml_diff>
--- a/examples/counters/DOAGC.xlsx
+++ b/examples/counters/DOAGC.xlsx
@@ -9,7 +9,6 @@
   </bookViews>
   <sheets>
     <sheet name="Counters" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="44">
   <si>
     <t xml:space="preserve">Nationality</t>
   </si>
@@ -153,27 +152,6 @@
   </si>
   <si>
     <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Army</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Attack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Move</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Designation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grouping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GAME TURN</t>
   </si>
 </sst>
 </file>
@@ -386,17 +364,18 @@
   </sheetPr>
   <dimension ref="A1:AMJ201"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B159" activeCellId="0" sqref="B159"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="LX1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="LX1" activeCellId="0" sqref="LX1"/>
+      <selection pane="bottomLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.35"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="647" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -421,6 +400,384 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="XR1" s="0"/>
+      <c r="XS1" s="0"/>
+      <c r="XT1" s="0"/>
+      <c r="XU1" s="0"/>
+      <c r="XV1" s="0"/>
+      <c r="XW1" s="0"/>
+      <c r="XX1" s="0"/>
+      <c r="XY1" s="0"/>
+      <c r="XZ1" s="0"/>
+      <c r="YA1" s="0"/>
+      <c r="YB1" s="0"/>
+      <c r="YC1" s="0"/>
+      <c r="YD1" s="0"/>
+      <c r="YE1" s="0"/>
+      <c r="YF1" s="0"/>
+      <c r="YG1" s="0"/>
+      <c r="YH1" s="0"/>
+      <c r="YI1" s="0"/>
+      <c r="YJ1" s="0"/>
+      <c r="YK1" s="0"/>
+      <c r="YL1" s="0"/>
+      <c r="YM1" s="0"/>
+      <c r="YN1" s="0"/>
+      <c r="YO1" s="0"/>
+      <c r="YP1" s="0"/>
+      <c r="YQ1" s="0"/>
+      <c r="YR1" s="0"/>
+      <c r="YS1" s="0"/>
+      <c r="YT1" s="0"/>
+      <c r="YU1" s="0"/>
+      <c r="YV1" s="0"/>
+      <c r="YW1" s="0"/>
+      <c r="YX1" s="0"/>
+      <c r="YY1" s="0"/>
+      <c r="YZ1" s="0"/>
+      <c r="ZA1" s="0"/>
+      <c r="ZB1" s="0"/>
+      <c r="ZC1" s="0"/>
+      <c r="ZD1" s="0"/>
+      <c r="ZE1" s="0"/>
+      <c r="ZF1" s="0"/>
+      <c r="ZG1" s="0"/>
+      <c r="ZH1" s="0"/>
+      <c r="ZI1" s="0"/>
+      <c r="ZJ1" s="0"/>
+      <c r="ZK1" s="0"/>
+      <c r="ZL1" s="0"/>
+      <c r="ZM1" s="0"/>
+      <c r="ZN1" s="0"/>
+      <c r="ZO1" s="0"/>
+      <c r="ZP1" s="0"/>
+      <c r="ZQ1" s="0"/>
+      <c r="ZR1" s="0"/>
+      <c r="ZS1" s="0"/>
+      <c r="ZT1" s="0"/>
+      <c r="ZU1" s="0"/>
+      <c r="ZV1" s="0"/>
+      <c r="ZW1" s="0"/>
+      <c r="ZX1" s="0"/>
+      <c r="ZY1" s="0"/>
+      <c r="ZZ1" s="0"/>
+      <c r="AAA1" s="0"/>
+      <c r="AAB1" s="0"/>
+      <c r="AAC1" s="0"/>
+      <c r="AAD1" s="0"/>
+      <c r="AAE1" s="0"/>
+      <c r="AAF1" s="0"/>
+      <c r="AAG1" s="0"/>
+      <c r="AAH1" s="0"/>
+      <c r="AAI1" s="0"/>
+      <c r="AAJ1" s="0"/>
+      <c r="AAK1" s="0"/>
+      <c r="AAL1" s="0"/>
+      <c r="AAM1" s="0"/>
+      <c r="AAN1" s="0"/>
+      <c r="AAO1" s="0"/>
+      <c r="AAP1" s="0"/>
+      <c r="AAQ1" s="0"/>
+      <c r="AAR1" s="0"/>
+      <c r="AAS1" s="0"/>
+      <c r="AAT1" s="0"/>
+      <c r="AAU1" s="0"/>
+      <c r="AAV1" s="0"/>
+      <c r="AAW1" s="0"/>
+      <c r="AAX1" s="0"/>
+      <c r="AAY1" s="0"/>
+      <c r="AAZ1" s="0"/>
+      <c r="ABA1" s="0"/>
+      <c r="ABB1" s="0"/>
+      <c r="ABC1" s="0"/>
+      <c r="ABD1" s="0"/>
+      <c r="ABE1" s="0"/>
+      <c r="ABF1" s="0"/>
+      <c r="ABG1" s="0"/>
+      <c r="ABH1" s="0"/>
+      <c r="ABI1" s="0"/>
+      <c r="ABJ1" s="0"/>
+      <c r="ABK1" s="0"/>
+      <c r="ABL1" s="0"/>
+      <c r="ABM1" s="0"/>
+      <c r="ABN1" s="0"/>
+      <c r="ABO1" s="0"/>
+      <c r="ABP1" s="0"/>
+      <c r="ABQ1" s="0"/>
+      <c r="ABR1" s="0"/>
+      <c r="ABS1" s="0"/>
+      <c r="ABT1" s="0"/>
+      <c r="ABU1" s="0"/>
+      <c r="ABV1" s="0"/>
+      <c r="ABW1" s="0"/>
+      <c r="ABX1" s="0"/>
+      <c r="ABY1" s="0"/>
+      <c r="ABZ1" s="0"/>
+      <c r="ACA1" s="0"/>
+      <c r="ACB1" s="0"/>
+      <c r="ACC1" s="0"/>
+      <c r="ACD1" s="0"/>
+      <c r="ACE1" s="0"/>
+      <c r="ACF1" s="0"/>
+      <c r="ACG1" s="0"/>
+      <c r="ACH1" s="0"/>
+      <c r="ACI1" s="0"/>
+      <c r="ACJ1" s="0"/>
+      <c r="ACK1" s="0"/>
+      <c r="ACL1" s="0"/>
+      <c r="ACM1" s="0"/>
+      <c r="ACN1" s="0"/>
+      <c r="ACO1" s="0"/>
+      <c r="ACP1" s="0"/>
+      <c r="ACQ1" s="0"/>
+      <c r="ACR1" s="0"/>
+      <c r="ACS1" s="0"/>
+      <c r="ACT1" s="0"/>
+      <c r="ACU1" s="0"/>
+      <c r="ACV1" s="0"/>
+      <c r="ACW1" s="0"/>
+      <c r="ACX1" s="0"/>
+      <c r="ACY1" s="0"/>
+      <c r="ACZ1" s="0"/>
+      <c r="ADA1" s="0"/>
+      <c r="ADB1" s="0"/>
+      <c r="ADC1" s="0"/>
+      <c r="ADD1" s="0"/>
+      <c r="ADE1" s="0"/>
+      <c r="ADF1" s="0"/>
+      <c r="ADG1" s="0"/>
+      <c r="ADH1" s="0"/>
+      <c r="ADI1" s="0"/>
+      <c r="ADJ1" s="0"/>
+      <c r="ADK1" s="0"/>
+      <c r="ADL1" s="0"/>
+      <c r="ADM1" s="0"/>
+      <c r="ADN1" s="0"/>
+      <c r="ADO1" s="0"/>
+      <c r="ADP1" s="0"/>
+      <c r="ADQ1" s="0"/>
+      <c r="ADR1" s="0"/>
+      <c r="ADS1" s="0"/>
+      <c r="ADT1" s="0"/>
+      <c r="ADU1" s="0"/>
+      <c r="ADV1" s="0"/>
+      <c r="ADW1" s="0"/>
+      <c r="ADX1" s="0"/>
+      <c r="ADY1" s="0"/>
+      <c r="ADZ1" s="0"/>
+      <c r="AEA1" s="0"/>
+      <c r="AEB1" s="0"/>
+      <c r="AEC1" s="0"/>
+      <c r="AED1" s="0"/>
+      <c r="AEE1" s="0"/>
+      <c r="AEF1" s="0"/>
+      <c r="AEG1" s="0"/>
+      <c r="AEH1" s="0"/>
+      <c r="AEI1" s="0"/>
+      <c r="AEJ1" s="0"/>
+      <c r="AEK1" s="0"/>
+      <c r="AEL1" s="0"/>
+      <c r="AEM1" s="0"/>
+      <c r="AEN1" s="0"/>
+      <c r="AEO1" s="0"/>
+      <c r="AEP1" s="0"/>
+      <c r="AEQ1" s="0"/>
+      <c r="AER1" s="0"/>
+      <c r="AES1" s="0"/>
+      <c r="AET1" s="0"/>
+      <c r="AEU1" s="0"/>
+      <c r="AEV1" s="0"/>
+      <c r="AEW1" s="0"/>
+      <c r="AEX1" s="0"/>
+      <c r="AEY1" s="0"/>
+      <c r="AEZ1" s="0"/>
+      <c r="AFA1" s="0"/>
+      <c r="AFB1" s="0"/>
+      <c r="AFC1" s="0"/>
+      <c r="AFD1" s="0"/>
+      <c r="AFE1" s="0"/>
+      <c r="AFF1" s="0"/>
+      <c r="AFG1" s="0"/>
+      <c r="AFH1" s="0"/>
+      <c r="AFI1" s="0"/>
+      <c r="AFJ1" s="0"/>
+      <c r="AFK1" s="0"/>
+      <c r="AFL1" s="0"/>
+      <c r="AFM1" s="0"/>
+      <c r="AFN1" s="0"/>
+      <c r="AFO1" s="0"/>
+      <c r="AFP1" s="0"/>
+      <c r="AFQ1" s="0"/>
+      <c r="AFR1" s="0"/>
+      <c r="AFS1" s="0"/>
+      <c r="AFT1" s="0"/>
+      <c r="AFU1" s="0"/>
+      <c r="AFV1" s="0"/>
+      <c r="AFW1" s="0"/>
+      <c r="AFX1" s="0"/>
+      <c r="AFY1" s="0"/>
+      <c r="AFZ1" s="0"/>
+      <c r="AGA1" s="0"/>
+      <c r="AGB1" s="0"/>
+      <c r="AGC1" s="0"/>
+      <c r="AGD1" s="0"/>
+      <c r="AGE1" s="0"/>
+      <c r="AGF1" s="0"/>
+      <c r="AGG1" s="0"/>
+      <c r="AGH1" s="0"/>
+      <c r="AGI1" s="0"/>
+      <c r="AGJ1" s="0"/>
+      <c r="AGK1" s="0"/>
+      <c r="AGL1" s="0"/>
+      <c r="AGM1" s="0"/>
+      <c r="AGN1" s="0"/>
+      <c r="AGO1" s="0"/>
+      <c r="AGP1" s="0"/>
+      <c r="AGQ1" s="0"/>
+      <c r="AGR1" s="0"/>
+      <c r="AGS1" s="0"/>
+      <c r="AGT1" s="0"/>
+      <c r="AGU1" s="0"/>
+      <c r="AGV1" s="0"/>
+      <c r="AGW1" s="0"/>
+      <c r="AGX1" s="0"/>
+      <c r="AGY1" s="0"/>
+      <c r="AGZ1" s="0"/>
+      <c r="AHA1" s="0"/>
+      <c r="AHB1" s="0"/>
+      <c r="AHC1" s="0"/>
+      <c r="AHD1" s="0"/>
+      <c r="AHE1" s="0"/>
+      <c r="AHF1" s="0"/>
+      <c r="AHG1" s="0"/>
+      <c r="AHH1" s="0"/>
+      <c r="AHI1" s="0"/>
+      <c r="AHJ1" s="0"/>
+      <c r="AHK1" s="0"/>
+      <c r="AHL1" s="0"/>
+      <c r="AHM1" s="0"/>
+      <c r="AHN1" s="0"/>
+      <c r="AHO1" s="0"/>
+      <c r="AHP1" s="0"/>
+      <c r="AHQ1" s="0"/>
+      <c r="AHR1" s="0"/>
+      <c r="AHS1" s="0"/>
+      <c r="AHT1" s="0"/>
+      <c r="AHU1" s="0"/>
+      <c r="AHV1" s="0"/>
+      <c r="AHW1" s="0"/>
+      <c r="AHX1" s="0"/>
+      <c r="AHY1" s="0"/>
+      <c r="AHZ1" s="0"/>
+      <c r="AIA1" s="0"/>
+      <c r="AIB1" s="0"/>
+      <c r="AIC1" s="0"/>
+      <c r="AID1" s="0"/>
+      <c r="AIE1" s="0"/>
+      <c r="AIF1" s="0"/>
+      <c r="AIG1" s="0"/>
+      <c r="AIH1" s="0"/>
+      <c r="AII1" s="0"/>
+      <c r="AIJ1" s="0"/>
+      <c r="AIK1" s="0"/>
+      <c r="AIL1" s="0"/>
+      <c r="AIM1" s="0"/>
+      <c r="AIN1" s="0"/>
+      <c r="AIO1" s="0"/>
+      <c r="AIP1" s="0"/>
+      <c r="AIQ1" s="0"/>
+      <c r="AIR1" s="0"/>
+      <c r="AIS1" s="0"/>
+      <c r="AIT1" s="0"/>
+      <c r="AIU1" s="0"/>
+      <c r="AIV1" s="0"/>
+      <c r="AIW1" s="0"/>
+      <c r="AIX1" s="0"/>
+      <c r="AIY1" s="0"/>
+      <c r="AIZ1" s="0"/>
+      <c r="AJA1" s="0"/>
+      <c r="AJB1" s="0"/>
+      <c r="AJC1" s="0"/>
+      <c r="AJD1" s="0"/>
+      <c r="AJE1" s="0"/>
+      <c r="AJF1" s="0"/>
+      <c r="AJG1" s="0"/>
+      <c r="AJH1" s="0"/>
+      <c r="AJI1" s="0"/>
+      <c r="AJJ1" s="0"/>
+      <c r="AJK1" s="0"/>
+      <c r="AJL1" s="0"/>
+      <c r="AJM1" s="0"/>
+      <c r="AJN1" s="0"/>
+      <c r="AJO1" s="0"/>
+      <c r="AJP1" s="0"/>
+      <c r="AJQ1" s="0"/>
+      <c r="AJR1" s="0"/>
+      <c r="AJS1" s="0"/>
+      <c r="AJT1" s="0"/>
+      <c r="AJU1" s="0"/>
+      <c r="AJV1" s="0"/>
+      <c r="AJW1" s="0"/>
+      <c r="AJX1" s="0"/>
+      <c r="AJY1" s="0"/>
+      <c r="AJZ1" s="0"/>
+      <c r="AKA1" s="0"/>
+      <c r="AKB1" s="0"/>
+      <c r="AKC1" s="0"/>
+      <c r="AKD1" s="0"/>
+      <c r="AKE1" s="0"/>
+      <c r="AKF1" s="0"/>
+      <c r="AKG1" s="0"/>
+      <c r="AKH1" s="0"/>
+      <c r="AKI1" s="0"/>
+      <c r="AKJ1" s="0"/>
+      <c r="AKK1" s="0"/>
+      <c r="AKL1" s="0"/>
+      <c r="AKM1" s="0"/>
+      <c r="AKN1" s="0"/>
+      <c r="AKO1" s="0"/>
+      <c r="AKP1" s="0"/>
+      <c r="AKQ1" s="0"/>
+      <c r="AKR1" s="0"/>
+      <c r="AKS1" s="0"/>
+      <c r="AKT1" s="0"/>
+      <c r="AKU1" s="0"/>
+      <c r="AKV1" s="0"/>
+      <c r="AKW1" s="0"/>
+      <c r="AKX1" s="0"/>
+      <c r="AKY1" s="0"/>
+      <c r="AKZ1" s="0"/>
+      <c r="ALA1" s="0"/>
+      <c r="ALB1" s="0"/>
+      <c r="ALC1" s="0"/>
+      <c r="ALD1" s="0"/>
+      <c r="ALE1" s="0"/>
+      <c r="ALF1" s="0"/>
+      <c r="ALG1" s="0"/>
+      <c r="ALH1" s="0"/>
+      <c r="ALI1" s="0"/>
+      <c r="ALJ1" s="0"/>
+      <c r="ALK1" s="0"/>
+      <c r="ALL1" s="0"/>
+      <c r="ALM1" s="0"/>
+      <c r="ALN1" s="0"/>
+      <c r="ALO1" s="0"/>
+      <c r="ALP1" s="0"/>
+      <c r="ALQ1" s="0"/>
+      <c r="ALR1" s="0"/>
+      <c r="ALS1" s="0"/>
+      <c r="ALT1" s="0"/>
+      <c r="ALU1" s="0"/>
+      <c r="ALV1" s="0"/>
+      <c r="ALW1" s="0"/>
+      <c r="ALX1" s="0"/>
+      <c r="ALY1" s="0"/>
+      <c r="ALZ1" s="0"/>
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
       <c r="AMF1" s="0"/>
       <c r="AMG1" s="0"/>
       <c r="AMH1" s="0"/>
@@ -4351,1957 +4708,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:G101"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G101" activeCellId="0" sqref="G101"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="3" style="1" width="11.52"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>29</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>31</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>35</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>36</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>38</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>39</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D11" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D12" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E14" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D15" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E15" s="1" t="n">
-        <v>43</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D16" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" s="1" t="n">
-        <v>44</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D17" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E17" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D18" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>46</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D19" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E19" s="1" t="n">
-        <v>47</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D20" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E20" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D21" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E21" s="1" t="n">
-        <v>49</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D22" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E22" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D23" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E23" s="5" t="n">
-        <v>51</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D24" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E24" s="5" t="n">
-        <v>52</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D25" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E25" s="5" t="n">
-        <v>53</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D26" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E26" s="5" t="n">
-        <v>54</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C27" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D27" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E27" s="5" t="n">
-        <v>55</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C28" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D28" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E28" s="5" t="n">
-        <v>56</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D29" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E29" s="5" t="n">
-        <v>57</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D30" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>58</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D31" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E31" s="5" t="n">
-        <v>59</v>
-      </c>
-      <c r="F31" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C32" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D32" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E32" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C33" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D33" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>61</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D34" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>62</v>
-      </c>
-      <c r="F34" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C35" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D35" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E35" s="1" t="n">
-        <v>63</v>
-      </c>
-      <c r="F35" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C36" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D36" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="F36" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C37" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D37" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E37" s="1" t="n">
-        <v>65</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D38" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E38" s="1" t="n">
-        <v>66</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D39" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E39" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D40" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E40" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C41" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D41" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E41" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D42" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E42" s="5" t="n">
-        <v>70</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D43" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E43" s="5" t="n">
-        <v>71</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D44" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E44" s="5" t="n">
-        <v>72</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C45" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D45" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E45" s="5" t="n">
-        <v>73</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C46" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D46" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E46" s="5" t="n">
-        <v>74</v>
-      </c>
-      <c r="F46" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D47" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E47" s="5" t="n">
-        <v>75</v>
-      </c>
-      <c r="F47" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C48" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D48" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E48" s="5" t="n">
-        <v>76</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C49" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D49" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E49" s="5" t="n">
-        <v>80</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C50" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D50" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E50" s="5" t="n">
-        <v>81</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D51" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E51" s="5" t="n">
-        <v>82</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E52" s="1" t="n">
-        <v>83</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E53" s="1" t="n">
-        <v>84</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D54" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E54" s="1" t="n">
-        <v>89</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C55" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D55" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E55" s="1" t="n">
-        <v>92</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C56" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D56" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E56" s="1" t="n">
-        <v>94</v>
-      </c>
-      <c r="F56" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B57" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C57" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D57" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E57" s="1" t="n">
-        <v>101</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B58" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C58" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E58" s="1" t="n">
-        <v>105</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B59" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D59" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B60" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D60" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E60" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D61" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E61" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D62" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E62" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C63" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D63" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F63" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C64" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D64" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E64" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F64" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C65" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D65" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C66" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D66" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E66" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C67" s="5" t="n">
-        <v>4</v>
-      </c>
-      <c r="D67" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E67" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C68" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D68" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E68" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F68" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C69" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D69" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E69" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F69" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D70" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E70" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F70" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C71" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D71" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="E71" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F71" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B72" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D72" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E72" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C73" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D73" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E73" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C74" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D74" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E74" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B75" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D75" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B76" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C76" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="D76" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="E76" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D77" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D78" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B79" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D79" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="E79" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F80" s="1"/>
-      <c r="G80" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F81" s="1"/>
-      <c r="G81" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C82" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D82" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E82" s="5" t="n">
-        <v>25</v>
-      </c>
-      <c r="F82" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B83" s="4"/>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
-      <c r="E84" s="5"/>
-      <c r="F84" s="5"/>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D85" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E85" s="5" t="n">
-        <v>131</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B86" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D86" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E86" s="5" t="n">
-        <v>367</v>
-      </c>
-      <c r="F86" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B87" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" s="5" t="n">
-        <v>2</v>
-      </c>
-      <c r="D87" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="E87" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="F87" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B88" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C88" s="5" t="n">
-        <v>5</v>
-      </c>
-      <c r="D88" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="E88" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="F88" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B89" s="4"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-      <c r="G89" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B90" s="4"/>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
-      <c r="E90" s="5"/>
-      <c r="F90" s="5"/>
-      <c r="G90" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B91" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C91" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D91" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B92" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C92" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D92" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B94" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C94" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="D94" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E94" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="F94" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B95" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D95" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E95" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F95" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B96" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C96" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D96" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E96" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="F96" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C97" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D97" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E97" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="F97" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B98" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C98" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="D98" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E98" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="F98" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G99" s="7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B100" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C100" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D100" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B101" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C101" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D101" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>